<commit_message>
Added color for Nwis flags
</commit_message>
<xml_diff>
--- a/C#/USGCExcelReader/Flags and Remark mappings.xlsx
+++ b/C#/USGCExcelReader/Flags and Remark mappings.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="10545"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="10485"/>
   </bookViews>
   <sheets>
-    <sheet name="AI Flags" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="82">
   <si>
     <t>Code</t>
   </si>
@@ -199,6 +199,69 @@
   </si>
   <si>
     <t>THIS VALUE RECIEVED FROM BACKUP RECORDER</t>
+  </si>
+  <si>
+    <t>#008040</t>
+  </si>
+  <si>
+    <t>#ff8040</t>
+  </si>
+  <si>
+    <t>#00ff00</t>
+  </si>
+  <si>
+    <t>#0080ff</t>
+  </si>
+  <si>
+    <t>#ff80c0</t>
+  </si>
+  <si>
+    <t>#8080c0</t>
+  </si>
+  <si>
+    <t>#ff0000</t>
+  </si>
+  <si>
+    <t>#800040</t>
+  </si>
+  <si>
+    <t>#00ffff</t>
+  </si>
+  <si>
+    <t>#004080</t>
+  </si>
+  <si>
+    <t>#ff8000</t>
+  </si>
+  <si>
+    <t>#0000ff</t>
+  </si>
+  <si>
+    <t>#0080c0</t>
+  </si>
+  <si>
+    <t>#808040</t>
+  </si>
+  <si>
+    <t>#008000</t>
+  </si>
+  <si>
+    <t>#8000ff</t>
+  </si>
+  <si>
+    <t>#80ff00</t>
+  </si>
+  <si>
+    <t>#804000</t>
+  </si>
+  <si>
+    <t>#80ff80</t>
+  </si>
+  <si>
+    <t>#ff80ff</t>
+  </si>
+  <si>
+    <t>#ff0080</t>
   </si>
 </sst>
 </file>
@@ -541,7 +604,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,6 +646,9 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
       <c r="E2" t="s">
         <v>33</v>
       </c>
@@ -600,6 +666,9 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
       <c r="E3" t="s">
         <v>33</v>
       </c>
@@ -617,6 +686,9 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
       <c r="E4" t="s">
         <v>33</v>
       </c>
@@ -633,6 +705,9 @@
       </c>
       <c r="C5" t="s">
         <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>33</v>
@@ -652,6 +727,9 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
       <c r="E6" t="s">
         <v>33</v>
       </c>
@@ -670,6 +748,9 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
       <c r="E7" t="s">
         <v>33</v>
       </c>
@@ -688,6 +769,9 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
       <c r="E8" t="s">
         <v>33</v>
       </c>
@@ -706,6 +790,9 @@
       <c r="C9" t="s">
         <v>13</v>
       </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
       <c r="E9" t="s">
         <v>33</v>
       </c>
@@ -724,6 +811,9 @@
       <c r="C10" t="s">
         <v>14</v>
       </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
       <c r="E10" t="s">
         <v>33</v>
       </c>
@@ -742,6 +832,9 @@
       <c r="C11" t="s">
         <v>15</v>
       </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
       <c r="E11" t="s">
         <v>33</v>
       </c>
@@ -760,6 +853,9 @@
       <c r="C12" t="s">
         <v>16</v>
       </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
       <c r="E12" t="s">
         <v>33</v>
       </c>
@@ -778,6 +874,9 @@
       <c r="C13" t="s">
         <v>17</v>
       </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
       <c r="E13" t="s">
         <v>33</v>
       </c>
@@ -796,6 +895,9 @@
       <c r="C14" t="s">
         <v>18</v>
       </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
       <c r="E14" t="s">
         <v>34</v>
       </c>
@@ -814,6 +916,9 @@
       <c r="C15" t="s">
         <v>19</v>
       </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
       <c r="E15" t="s">
         <v>35</v>
       </c>
@@ -832,6 +937,9 @@
       <c r="C16" t="s">
         <v>23</v>
       </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
       <c r="E16" t="s">
         <v>36</v>
       </c>
@@ -850,6 +958,9 @@
       <c r="C17" t="s">
         <v>24</v>
       </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
       <c r="E17" t="s">
         <v>36</v>
       </c>
@@ -868,6 +979,9 @@
       <c r="C18" t="s">
         <v>25</v>
       </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
       <c r="E18" t="s">
         <v>36</v>
       </c>
@@ -886,6 +1000,9 @@
       <c r="C19" t="s">
         <v>26</v>
       </c>
+      <c r="D19" t="s">
+        <v>77</v>
+      </c>
       <c r="E19" t="s">
         <v>36</v>
       </c>
@@ -904,6 +1021,9 @@
       <c r="C20" t="s">
         <v>27</v>
       </c>
+      <c r="D20" t="s">
+        <v>78</v>
+      </c>
       <c r="E20" t="s">
         <v>36</v>
       </c>
@@ -922,6 +1042,9 @@
       <c r="C21" t="s">
         <v>28</v>
       </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
       <c r="E21" t="s">
         <v>36</v>
       </c>
@@ -940,6 +1063,9 @@
       <c r="C22" t="s">
         <v>29</v>
       </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
       <c r="E22" t="s">
         <v>36</v>
       </c>
@@ -958,6 +1084,9 @@
       <c r="C23" t="s">
         <v>30</v>
       </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
       <c r="E23" t="s">
         <v>36</v>
       </c>
@@ -976,6 +1105,9 @@
       <c r="C24" t="s">
         <v>31</v>
       </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
       <c r="E24" t="s">
         <v>36</v>
       </c>
@@ -993,6 +1125,9 @@
       </c>
       <c r="C25" t="s">
         <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>81</v>
       </c>
       <c r="E25" t="s">
         <v>36</v>

</xml_diff>